<commit_message>
Add binnacle to doc and update graphs
</commit_message>
<xml_diff>
--- a/graphs/graphs.xlsx
+++ b/graphs/graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Java\algorithm-analysis-p2\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC7EE5F-F601-493B-9AFF-DBD706F243F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1BDAD6-C6D0-4BAC-9582-01D62E7BAFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4FEC4A4F-953F-4A07-8A1B-3052437AD2D7}"/>
   </bookViews>
@@ -842,6 +842,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -903,6 +958,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Datos</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> consumidos</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1444,6 +1559,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1505,6 +1675,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Datos</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> consumidos</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2171,6 +2401,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2232,6 +2517,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Datos consumidos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2714,6 +3054,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2775,6 +3170,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Asignaciones realizadas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3259,6 +3709,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3320,6 +3825,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Comparaciones</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> realizadas</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3802,6 +4367,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3863,6 +4483,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Instrucciones realizadas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4345,6 +5020,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4406,6 +5136,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de ejecucion</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4883,6 +5673,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Archivo</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4944,6 +5789,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memoria</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> consumida</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -9562,10 +10467,10 @@
       <xdr:rowOff>839</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>295836</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>94408</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10108,8 +11013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315CE844-F26E-4629-ACFC-739C1DBF0D2C}">
   <dimension ref="B1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S78" sqref="S78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>